<commit_message>
new status for url shortner and notification system
</commit_message>
<xml_diff>
--- a/HLD.xlsx
+++ b/HLD.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5cfd33913750facc/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobs4\Intellij\PrepTracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A99D8BD-1CF3-4537-89B2-88E42D0ED6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842C384D-7FC8-4968-B23D-FC12A9541337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DFC65BCF-6B0B-4691-A374-E716F295FFA4}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,12 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t xml:space="preserve">Topic </t>
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Notification System</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>URL Shortner</t>
   </si>
 </sst>
 </file>
@@ -393,13 +400,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{042B1DFE-1CFF-42B4-A26F-49FC90DF550F}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -407,6 +417,22 @@
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>